<commit_message>
update result 20201207 & update plan 20201208
</commit_message>
<xml_diff>
--- a/20201207.xlsx
+++ b/20201207.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FE5799-AC74-4069-9D01-50AF8BAA1ECB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C76D28-D3B4-4963-A9C3-51DFED4A3685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>일</t>
   </si>
@@ -226,6 +226,16 @@
   <si>
     <t>1. 월수금 지키기
 2. 아침공부 하기</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. F7
+ - cp stat '9' 관련 내용 클리어
+ - 타임아웃 이슈 : 갑자기 서버의 응답속도가 느려져서 기존 반응속도(5초)로 사용하니, 너무 타임아
+   웃이 자주 일어나고, 응답이 여러번겹쳐서 들어왔음 (타임아웃되고 packet을 재전송한 것까지 한
+   번에 응답으로 들어옴)
+  - 확인안된 사항 : 위 경우와 겹쳐서 hardfault가 나왔었음. 
+  - 로컬 때 저장한 패킷 전송 시 파일 포인터를 ROM에 저장</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -399,7 +409,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -601,6 +611,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -907,7 +941,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,30 +954,6 @@
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -971,21 +981,6 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -995,7 +990,64 @@
     <xf numFmtId="176" fontId="1" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1530,8 +1582,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1594,25 +1646,27 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="26" t="s">
+      <c r="F3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="18" t="s">
+      <c r="H3" s="33"/>
+      <c r="I3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="12"/>
+      <c r="J3" s="4"/>
       <c r="K3" t="s">
         <v>13</v>
       </c>
@@ -1624,15 +1678,15 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="13"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="5"/>
       <c r="K4" t="s">
         <v>11</v>
       </c>
@@ -1641,15 +1695,15 @@
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="13"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="5"/>
       <c r="K5" t="s">
         <v>12</v>
       </c>
@@ -1658,15 +1712,15 @@
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="13"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="5"/>
       <c r="K6" t="s">
         <v>10</v>
       </c>
@@ -1675,15 +1729,15 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="13"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="5"/>
       <c r="K7" t="s">
         <v>8</v>
       </c>
@@ -1696,15 +1750,15 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="13"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="5"/>
       <c r="K8" t="s">
         <v>4</v>
       </c>
@@ -1713,244 +1767,244 @@
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="13"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="13"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="13"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="13"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:15" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="13"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="13"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="13"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:10" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="13"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="13"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="13"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="13"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="14"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="G3:G23"/>
+    <mergeCell ref="D3:D8"/>
     <mergeCell ref="J3:J23"/>
     <mergeCell ref="H3:H23"/>
     <mergeCell ref="E3:E23"/>
     <mergeCell ref="I3:I23"/>
     <mergeCell ref="F3:F23"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="G3:G23"/>
-    <mergeCell ref="D3:D8"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>